<commit_message>
Support for question types and implementing various tkinter input types
</commit_message>
<xml_diff>
--- a/food_log.xlsx
+++ b/food_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -600,6 +600,97 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-12-12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-12-13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Option 3</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-12-13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sdasd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sdsds</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Option 2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
+ fixed window size
</commit_message>
<xml_diff>
--- a/food_log.xlsx
+++ b/food_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,15 +835,51 @@
           <t>12/13/2024</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
           <t>Item 1,Item 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>12/1/2024</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>this is a link</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>dish name</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Sheet Pan</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Tasted amazing</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Item 1,Item 4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Exception / Error handling and more dynamic handling of value inputs for the questions
</commit_message>
<xml_diff>
--- a/food_log.xlsx
+++ b/food_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,13 +479,59 @@
           <t>dddd</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>Holds well in Fridge,Does not hold well in Fridge</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12/14/2024</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Missing Options!</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>wqew</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Freezes well,Freezes Poorly,Holds well in Fridge</t>
         </is>
       </c>
     </row>

</xml_diff>